<commit_message>
added all source country data and updated relevant do files to prepare and combine all origin country data
</commit_message>
<xml_diff>
--- a/src/original_data/help/list_of_origin_countries.xlsx
+++ b/src/original_data/help/list_of_origin_countries.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Iraq</t>
   </si>
@@ -193,9 +193,6 @@
   </si>
   <si>
     <t>Togo</t>
-  </si>
-  <si>
-    <t>Palestine</t>
   </si>
   <si>
     <t>Senegal</t>
@@ -541,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A62"/>
+  <dimension ref="A1:A61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,102 +760,97 @@
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>59</v>
+      <c r="A43" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>41</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>2</v>
+      <c r="A45" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>57</v>
+      <c r="A46" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>60</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>47</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>1</v>
+      <c r="A54" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>61</v>
+      <c r="A56" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed decision baseline sample to no longer include Bulgaria and Malta. Created decision country samples with few and early elections.
</commit_message>
<xml_diff>
--- a/src/original_data/help/list_of_origin_countries.xlsx
+++ b/src/original_data/help/list_of_origin_countries.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Iraq</t>
   </si>
@@ -199,6 +199,12 @@
   </si>
   <si>
     <t>Tunisia</t>
+  </si>
+  <si>
+    <t>Comoros</t>
+  </si>
+  <si>
+    <t>Kazakhstan</t>
   </si>
 </sst>
 </file>
@@ -538,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A61"/>
+  <dimension ref="A1:A63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,6 +858,16 @@
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>